<commit_message>
change in movements and progess in validations
</commit_message>
<xml_diff>
--- a/bootcampp/bootcamp.xlsx
+++ b/bootcampp/bootcamp.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carga\Desktop\p_bootcamp\bootcampp\diagrama\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wverague\Desktop\semana2\bootcamp-1\bootcampp\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E066150-7D9F-4458-A220-8AA84EBB3281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,19 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>CLIENTES</t>
   </si>
@@ -136,12 +130,63 @@
   </si>
   <si>
     <t>fechaRegistro</t>
+  </si>
+  <si>
+    <t>TRANSFERENCIAS</t>
+  </si>
+  <si>
+    <t>REPORTE</t>
+  </si>
+  <si>
+    <t>tipo(interna, externo)</t>
+  </si>
+  <si>
+    <t>monto_diario</t>
+  </si>
+  <si>
+    <t>id_cta_origen</t>
+  </si>
+  <si>
+    <t>c_comicion</t>
+  </si>
+  <si>
+    <t>id_cta_destino</t>
+  </si>
+  <si>
+    <t>id_trasferencia</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>idcuentabancaria</t>
+  </si>
+  <si>
+    <t>PERFILES</t>
+  </si>
+  <si>
+    <t>tipo(VIP, PIME)</t>
+  </si>
+  <si>
+    <t>montomin</t>
+  </si>
+  <si>
+    <t>idPerfil</t>
+  </si>
+  <si>
+    <t>monto_min_mes</t>
+  </si>
+  <si>
+    <t>lim_max_mov</t>
+  </si>
+  <si>
+    <t>montoMax</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -151,7 +196,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,6 +212,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC65911"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -278,6 +329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -301,13 +353,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -315,7 +367,7 @@
         <xdr:cNvPr id="5" name="Conector recto de flecha 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{857E7C96-EA1C-425C-853E-A1D249806ED9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{857E7C96-EA1C-425C-853E-A1D249806ED9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -368,7 +420,7 @@
         <xdr:cNvPr id="16" name="Conector recto de flecha 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BBECB934-FDC6-41D6-9011-1CBD731A41DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBECB934-FDC6-41D6-9011-1CBD731A41DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -407,13 +459,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -421,7 +473,7 @@
         <xdr:cNvPr id="18" name="Conector recto de flecha 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F2287DC0-B4A3-46DE-BF4A-24E29B6EBDCB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2287DC0-B4A3-46DE-BF4A-24E29B6EBDCB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -474,7 +526,7 @@
         <xdr:cNvPr id="15" name="Conector recto de flecha 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9C40F9FF-98C5-4FED-9660-219CE101BD9C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C40F9FF-98C5-4FED-9660-219CE101BD9C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -527,7 +579,7 @@
         <xdr:cNvPr id="19" name="Conector recto de flecha 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B61275D8-8248-4E62-9343-763C6EEEB8EB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B61275D8-8248-4E62-9343-763C6EEEB8EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -580,7 +632,7 @@
         <xdr:cNvPr id="21" name="Conector recto de flecha 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{949FD700-9DAD-4333-BF88-CE02AEBE7C7C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{949FD700-9DAD-4333-BF88-CE02AEBE7C7C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -619,13 +671,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -633,7 +685,7 @@
         <xdr:cNvPr id="17" name="Conector recto de flecha 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00269AE6-4197-414A-A1F2-4111839CB434}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00269AE6-4197-414A-A1F2-4111839CB434}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -643,6 +695,117 @@
         <a:xfrm flipH="1">
           <a:off x="3733800" y="7467600"/>
           <a:ext cx="695325" cy="704850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Conector recto de flecha 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6EB1FF4-0029-40F2-8647-D470056F32D8}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{00269AE6-4197-414A-A1F2-4111839CB434}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7033260" y="8180070"/>
+          <a:ext cx="1165860" cy="251460"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>948690</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Conector recto de flecha 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AA88A10-F3A4-485A-AC8F-C34F1F6E28EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2125980" y="1295400"/>
+          <a:ext cx="1550670" cy="937260"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -967,98 +1130,112 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D5" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="8"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
+      <c r="B15" s="12" t="s">
+        <v>48</v>
+      </c>
       <c r="C15" s="13"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1067,7 +1244,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7" t="s">
@@ -1078,7 +1255,7 @@
       <c r="F21" s="6"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1087,7 +1264,7 @@
       <c r="F22" s="6"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="9"/>
@@ -1096,7 +1273,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="9"/>
@@ -1105,7 +1282,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="9"/>
@@ -1114,7 +1291,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1123,7 +1300,7 @@
       <c r="F26" s="6"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1132,7 +1309,7 @@
       <c r="F27" s="6"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1141,7 +1318,7 @@
       <c r="F28" s="6"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1150,7 +1327,7 @@
       <c r="F29" s="6"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1159,7 +1336,7 @@
       <c r="F30" s="6"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="6" t="s">
         <v>27</v>
@@ -1172,7 +1349,7 @@
       </c>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="10" t="s">
         <v>11</v>
@@ -1187,7 +1364,7 @@
       </c>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="6" t="s">
         <v>6</v>
@@ -1202,7 +1379,7 @@
       </c>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="6" t="s">
         <v>16</v>
@@ -1220,7 +1397,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="6" t="s">
         <v>21</v>
@@ -1238,7 +1415,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="6" t="s">
         <v>12</v>
@@ -1256,137 +1433,200 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
-      <c r="B37" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="B37" s="6"/>
       <c r="C37" s="6"/>
-      <c r="D37" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G37" s="8"/>
-      <c r="I37" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
-      <c r="B38" s="6"/>
+      <c r="B38" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
+      <c r="D38" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="E38" s="6"/>
       <c r="F38" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="8"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
-      <c r="F39" s="6" t="s">
+      <c r="F39" t="s">
+        <v>49</v>
+      </c>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="5"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" t="s">
+        <v>50</v>
+      </c>
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="5"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" t="s">
+        <v>51</v>
+      </c>
+      <c r="G41" s="8"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="11"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G39" s="8"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="13"/>
-      <c r="I40" t="s">
+      <c r="G42" s="13"/>
+      <c r="I42" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I41" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I43" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I42" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I44" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C43" s="2"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="4"/>
-      <c r="I43" t="s">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C45" s="2"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="4"/>
+      <c r="I45" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C44" s="5"/>
-      <c r="D44" s="10" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C46" s="5"/>
+      <c r="D46" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="8"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C45" s="5"/>
-      <c r="D45" s="9" t="s">
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C47" s="5"/>
+      <c r="D47" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E45" s="8"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C46" s="5"/>
-      <c r="D46" s="9" t="s">
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C48" s="5"/>
+      <c r="D48" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E46" s="8"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C47" s="5"/>
-      <c r="D47" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E47" s="8"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C48" s="5"/>
-      <c r="D48" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="E48" s="8"/>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G48" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J48" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C49" s="5"/>
       <c r="D49" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" s="8"/>
+      <c r="G49" t="s">
+        <v>6</v>
+      </c>
+      <c r="J49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C50" s="5"/>
+      <c r="D50" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" s="8"/>
+      <c r="G50" t="s">
+        <v>37</v>
+      </c>
+      <c r="J50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C51" s="5"/>
+      <c r="D51" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E49" s="8"/>
-    </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C50" s="5"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="8"/>
-    </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C51" s="5"/>
-      <c r="D51" s="6"/>
       <c r="E51" s="8"/>
-    </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>39</v>
+      </c>
+      <c r="J51" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C52" s="5"/>
       <c r="D52" s="6"/>
       <c r="E52" s="8"/>
-    </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C53" s="11"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="13"/>
+      <c r="G52" t="s">
+        <v>41</v>
+      </c>
+      <c r="J52" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C53" s="5"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="8"/>
+      <c r="G53" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C54" s="5"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="8"/>
+      <c r="G54" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C55" s="11"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="13"/>
+      <c r="G55" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>